<commit_message>
version prueba bot smelpro tareas
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SMELPRO\PROYECTOS\BOT_TAREAS_SMELPRO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\ahlely18\BOT_TAREAS_SMELPRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79200C5D-1994-4924-840F-B4F0D847B8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AE9E99-F554-49A1-8234-D5B2FF744EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{8C5C8D55-94B0-46BB-B24B-9AE00C92E136}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{8C5C8D55-94B0-46BB-B24B-9AE00C92E136}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -81,6 +81,42 @@
   </si>
   <si>
     <t>HORA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>@fiamahle</t>
+  </si>
+  <si>
+    <t>@cesar_sanchez_10</t>
+  </si>
+  <si>
+    <t>@diego_roca</t>
+  </si>
+  <si>
+    <t>@alexander0266</t>
+  </si>
+  <si>
+    <t>@Ozymandias_96</t>
+  </si>
+  <si>
+    <t>@DenisBT45</t>
+  </si>
+  <si>
+    <t>@HenryMera</t>
+  </si>
+  <si>
+    <t>@IsaFlores04</t>
+  </si>
+  <si>
+    <t>@YajaGVargas</t>
+  </si>
+  <si>
+    <t>@carlitavot</t>
+  </si>
+  <si>
+    <t>LIMPIAR MICROONDAS Y REFRIGERADORA</t>
   </si>
 </sst>
 </file>
@@ -454,166 +490,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4D38A3-6645-4965-B16A-ABEE6DD5806B}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E13" sqref="E13:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1">
-        <v>45975</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45980</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
         <v>45982</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
         <v>45987</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
         <v>45989</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45975</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.43819444444444444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45994</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1">
         <v>45996</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
         <v>46001</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1">
         <v>46003</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
         <v>46008</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
         <v>46010</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.72916666666666663</v>
+      <c r="E11" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45975</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1">
+        <v>46010</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45982</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45987</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45989</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45996</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1">
+        <v>46001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1">
+        <v>46003</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46008</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <v>46010</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>